<commit_message>
analysis: imgaug features presentation notebook
Added a new notebook under folder 'analysis' presenting
different features of library 'imgaug' that are used
in training.
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3042c0b8b0f90a7e/programming/AI/cursos/udacity/cnn-dog-breed-classifier/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="195" documentId="8_{8ADC6170-C625-4EE8-B519-94970A88485A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E6EC3423-34FD-41F2-A52A-EA76CAC3B45D}"/>
+  <xr:revisionPtr revIDLastSave="196" documentId="8_{8ADC6170-C625-4EE8-B519-94970A88485A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{04355E93-55FA-124F-B94F-47BAA4413C41}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{B07A66A9-E150-42D2-88E6-A6155F8A69BE}"/>
+    <workbookView xWindow="59280" yWindow="3120" windowWidth="38640" windowHeight="21400" activeTab="1" xr2:uid="{B07A66A9-E150-42D2-88E6-A6155F8A69BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="50">
   <si>
     <t>Problem:</t>
   </si>
@@ -415,9 +415,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Check Cell" xfId="4" builtinId="23"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Input" xfId="3" builtinId="20"/>
+    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
+    <cellStyle name="Celda de comprobación" xfId="4" builtinId="23"/>
+    <cellStyle name="Entrada" xfId="3" builtinId="20"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -462,7 +462,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -764,12 +764,12 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -777,7 +777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -785,7 +785,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -793,7 +793,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -801,43 +801,43 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
     </row>
   </sheetData>
@@ -848,38 +848,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B55D56D3-F049-4ABE-9A96-1854F8234D97}">
-  <dimension ref="A1:S50"/>
+  <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.5703125" customWidth="1"/>
-    <col min="14" max="14" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.5" customWidth="1"/>
+    <col min="14" max="14" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -887,13 +887,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>31</v>
       </c>
@@ -901,7 +901,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>32</v>
       </c>
@@ -909,7 +909,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>34</v>
       </c>
@@ -917,8 +917,8 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:19" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>28</v>
       </c>
@@ -977,7 +977,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>0.48</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>0.5</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>0.42</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>0.35</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="9" t="s">
         <v>38</v>
@@ -1270,7 +1270,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>0.49</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" s="12" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>0.57999999999999996</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>0.46</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>0.41</v>
       </c>
@@ -1506,7 +1506,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <v>0.31</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>0.45</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <v>0.32</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <v>0.44</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <v>0.47</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
         <v>0.43</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="5"/>
       <c r="B26" s="9" t="s">
         <v>29</v>
@@ -1917,7 +1917,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>0.54</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="5"/>
       <c r="B28" s="9" t="s">
         <v>29</v>
@@ -2033,1262 +2033,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H29" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I29" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J29" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K29" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L29" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M29" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N29" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O29" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P29" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q29" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R29" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S29" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G30" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I30" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J30" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K30" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L30" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M30" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N30" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O30" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P30" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q30" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R30" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S30" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H31" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I31" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J31" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K31" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L31" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M31" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N31" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O31" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P31" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q31" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R31" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S31" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I32" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J32" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K32" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L32" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M32" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N32" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O32" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P32" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q32" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R32" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S32" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H33" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J33" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K33" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L33" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M33" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N33" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O33" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P33" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q33" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R33" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S33" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G34" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I34" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J34" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K34" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L34" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M34" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N34" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O34" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P34" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q34" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R34" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S34" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G35" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I35" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J35" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K35" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L35" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M35" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N35" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O35" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P35" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q35" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R35" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S35" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I36" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J36" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K36" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L36" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M36" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N36" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O36" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P36" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q36" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R36" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S36" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F37" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G37" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I37" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J37" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K37" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L37" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M37" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N37" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O37" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P37" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q37" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R37" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S37" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G38" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H38" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I38" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J38" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K38" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L38" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M38" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N38" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O38" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P38" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q38" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R38" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S38" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F39" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G39" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H39" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I39" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J39" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K39" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L39" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M39" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N39" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O39" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P39" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q39" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R39" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S39" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F40" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G40" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H40" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I40" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J40" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K40" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L40" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M40" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N40" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O40" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P40" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q40" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R40" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S40" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G41" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H41" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I41" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J41" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K41" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L41" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M41" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N41" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O41" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P41" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q41" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R41" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S41" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G42" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H42" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I42" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J42" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K42" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L42" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M42" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N42" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O42" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P42" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q42" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R42" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S42" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-      <c r="B43" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F43" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G43" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H43" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I43" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J43" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K43" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L43" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M43" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N43" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O43" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P43" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q43" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R43" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S43" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F44" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G44" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H44" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I44" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J44" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K44" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L44" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M44" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N44" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O44" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P44" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q44" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R44" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S44" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F45" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G45" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H45" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I45" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J45" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K45" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L45" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M45" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N45" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O45" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P45" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q45" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R45" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S45" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F46" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G46" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H46" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I46" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J46" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K46" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L46" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M46" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N46" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O46" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P46" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q46" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R46" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S46" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E47" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F47" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G47" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H47" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I47" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J47" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K47" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L47" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M47" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N47" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O47" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P47" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q47" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R47" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S47" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D48" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F48" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G48" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H48" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I48" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J48" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K48" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L48" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M48" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N48" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O48" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P48" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q48" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R48" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S48" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-      <c r="B49" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F49" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G49" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H49" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I49" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J49" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K49" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L49" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M49" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N49" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O49" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P49" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q49" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R49" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S49" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
-      <c r="B50" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D50" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E50" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F50" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G50" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H50" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I50" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J50" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K50" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L50" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M50" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N50" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O50" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P50" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q50" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R50" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S50" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B11:S50">
+  <conditionalFormatting sqref="B11:S28">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="between">
       <formula>0</formula>
       <formula>1000</formula>
@@ -3315,7 +2061,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>B11:S50</xm:sqref>
+          <xm:sqref>B11:S28</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>